<commit_message>
Neuschreiben der Konfiguration für JMapper entfernt
</commit_message>
<xml_diff>
--- a/bean-mapper-test/docs/jdk8-03/PerformanceTestWithCompleteFixtures.xlsx
+++ b/bean-mapper-test/docs/jdk8-03/PerformanceTestWithCompleteFixtures.xlsx
@@ -15,7 +15,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="16">
   <si>
-    <t>05.05.2016 um 20:17 Uhr</t>
+    <t>05.05.2016 um 21:52 Uhr</t>
   </si>
   <si>
     <t>Name des Messpunkts</t>
@@ -164,7 +164,7 @@
         <v>10.0</v>
       </c>
       <c r="C3" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="D3" t="n">
         <v>0.0</v>
@@ -173,10 +173,10 @@
         <v>2.0</v>
       </c>
       <c r="F3" t="n" s="2">
-        <v>0.4</v>
+        <v>0.3</v>
       </c>
       <c r="G3" t="n" s="2">
-        <v>0.699206</v>
+        <v>0.674949</v>
       </c>
       <c r="H3" t="n">
         <v>0.0</v>
@@ -190,19 +190,19 @@
         <v>10.0</v>
       </c>
       <c r="C4" t="n">
-        <v>593.0</v>
+        <v>630.0</v>
       </c>
       <c r="D4" t="n">
-        <v>27.0</v>
+        <v>26.0</v>
       </c>
       <c r="E4" t="n">
-        <v>259.0</v>
+        <v>212.0</v>
       </c>
       <c r="F4" t="n" s="2">
-        <v>59.3</v>
+        <v>63.0</v>
       </c>
       <c r="G4" t="n" s="2">
-        <v>71.2025</v>
+        <v>56.1169</v>
       </c>
       <c r="H4" t="n">
         <v>27.0</v>
@@ -216,22 +216,22 @@
         <v>10.0</v>
       </c>
       <c r="C5" t="n">
-        <v>155.0</v>
+        <v>129.0</v>
       </c>
       <c r="D5" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
       <c r="E5" t="n">
-        <v>114.0</v>
+        <v>88.0</v>
       </c>
       <c r="F5" t="n" s="2">
-        <v>15.5</v>
+        <v>12.9</v>
       </c>
       <c r="G5" t="n" s="2">
-        <v>34.6546</v>
+        <v>26.451</v>
       </c>
       <c r="H5" t="n">
-        <v>2.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="6">
@@ -242,19 +242,19 @@
         <v>10.0</v>
       </c>
       <c r="C6" t="n">
-        <v>11.0</v>
+        <v>13.0</v>
       </c>
       <c r="D6" t="n">
         <v>0.0</v>
       </c>
       <c r="E6" t="n">
-        <v>4.0</v>
+        <v>3.0</v>
       </c>
       <c r="F6" t="n" s="2">
-        <v>1.1</v>
+        <v>1.3</v>
       </c>
       <c r="G6" t="n" s="2">
-        <v>1.19722</v>
+        <v>0.823273</v>
       </c>
       <c r="H6" t="n">
         <v>1.0</v>
@@ -268,22 +268,22 @@
         <v>10.0</v>
       </c>
       <c r="C7" t="n">
-        <v>462.0</v>
+        <v>508.0</v>
       </c>
       <c r="D7" t="n">
-        <v>13.0</v>
+        <v>15.0</v>
       </c>
       <c r="E7" t="n">
-        <v>253.0</v>
+        <v>256.0</v>
       </c>
       <c r="F7" t="n" s="2">
-        <v>46.2</v>
+        <v>50.8</v>
       </c>
       <c r="G7" t="n" s="2">
-        <v>73.1358</v>
+        <v>73.3285</v>
       </c>
       <c r="H7" t="n">
-        <v>17.0</v>
+        <v>23.0</v>
       </c>
     </row>
     <row r="8">
@@ -297,19 +297,19 @@
         <v>10.0</v>
       </c>
       <c r="D8" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
       <c r="E8" t="n">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="F8" t="n" s="2">
         <v>1.0</v>
       </c>
       <c r="G8" t="n" s="2">
-        <v>0.0</v>
+        <v>0.471405</v>
       </c>
       <c r="H8" t="n">
-        <v>1.0</v>
+        <v>0.0</v>
       </c>
     </row>
   </sheetData>
@@ -364,22 +364,22 @@
         <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>33181.0</v>
+        <v>32939.0</v>
       </c>
       <c r="C3" t="n">
-        <v>564.0</v>
+        <v>541.0</v>
       </c>
       <c r="D3" t="n">
         <v>0.0</v>
       </c>
       <c r="E3" t="n">
-        <v>3.0</v>
+        <v>6.0</v>
       </c>
       <c r="F3" t="n" s="2">
-        <v>0.0169977</v>
+        <v>0.0164243</v>
       </c>
       <c r="G3" t="n" s="2">
-        <v>0.131116</v>
+        <v>0.133396</v>
       </c>
       <c r="H3" t="n">
         <v>0.0</v>
@@ -390,22 +390,22 @@
         <v>10</v>
       </c>
       <c r="B4" t="n">
-        <v>33181.0</v>
+        <v>32939.0</v>
       </c>
       <c r="C4" t="n">
-        <v>370416.0</v>
+        <v>366885.0</v>
       </c>
       <c r="D4" t="n">
         <v>10.0</v>
       </c>
       <c r="E4" t="n">
-        <v>64.0</v>
+        <v>57.0</v>
       </c>
       <c r="F4" t="n" s="2">
-        <v>11.1635</v>
+        <v>11.1383</v>
       </c>
       <c r="G4" t="n" s="2">
-        <v>1.27571</v>
+        <v>1.32497</v>
       </c>
       <c r="H4" t="n">
         <v>11.0</v>
@@ -416,25 +416,25 @@
         <v>11</v>
       </c>
       <c r="B5" t="n">
-        <v>33181.0</v>
+        <v>32939.0</v>
       </c>
       <c r="C5" t="n">
-        <v>17938.0</v>
+        <v>17482.0</v>
       </c>
       <c r="D5" t="n">
         <v>0.0</v>
       </c>
       <c r="E5" t="n">
-        <v>15.0</v>
+        <v>37.0</v>
       </c>
       <c r="F5" t="n" s="2">
-        <v>0.540611</v>
+        <v>0.530739</v>
       </c>
       <c r="G5" t="n" s="2">
-        <v>0.527271</v>
+        <v>0.557399</v>
       </c>
       <c r="H5" t="n">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
     </row>
     <row r="6">
@@ -442,22 +442,22 @@
         <v>12</v>
       </c>
       <c r="B6" t="n">
-        <v>33181.0</v>
+        <v>32939.0</v>
       </c>
       <c r="C6" t="n">
-        <v>5439.0</v>
+        <v>5700.0</v>
       </c>
       <c r="D6" t="n">
         <v>0.0</v>
       </c>
       <c r="E6" t="n">
-        <v>15.0</v>
+        <v>12.0</v>
       </c>
       <c r="F6" t="n" s="2">
-        <v>0.163919</v>
+        <v>0.173047</v>
       </c>
       <c r="G6" t="n" s="2">
-        <v>0.386069</v>
+        <v>0.388118</v>
       </c>
       <c r="H6" t="n">
         <v>0.0</v>
@@ -468,22 +468,22 @@
         <v>13</v>
       </c>
       <c r="B7" t="n">
-        <v>33181.0</v>
+        <v>32939.0</v>
       </c>
       <c r="C7" t="n">
-        <v>181726.0</v>
+        <v>185247.0</v>
       </c>
       <c r="D7" t="n">
         <v>5.0</v>
       </c>
       <c r="E7" t="n">
-        <v>35.0</v>
+        <v>31.0</v>
       </c>
       <c r="F7" t="n" s="2">
-        <v>5.47681</v>
+        <v>5.62394</v>
       </c>
       <c r="G7" t="n" s="2">
-        <v>0.933461</v>
+        <v>0.964435</v>
       </c>
       <c r="H7" t="n">
         <v>5.0</v>
@@ -494,10 +494,10 @@
         <v>14</v>
       </c>
       <c r="B8" t="n">
-        <v>33181.0</v>
+        <v>32939.0</v>
       </c>
       <c r="C8" t="n">
-        <v>494.0</v>
+        <v>493.0</v>
       </c>
       <c r="D8" t="n">
         <v>0.0</v>
@@ -506,10 +506,10 @@
         <v>3.0</v>
       </c>
       <c r="F8" t="n" s="2">
-        <v>0.014888</v>
+        <v>0.0149671</v>
       </c>
       <c r="G8" t="n" s="2">
-        <v>0.123081</v>
+        <v>0.122667</v>
       </c>
       <c r="H8" t="n">
         <v>0.0</v>
@@ -546,19 +546,19 @@
         <v>0.1</v>
       </c>
       <c r="C12" t="n" s="2">
-        <v>0.05</v>
+        <v>0.03</v>
       </c>
       <c r="D12" t="n" s="2">
-        <v>0.02</v>
+        <v>0.016</v>
       </c>
       <c r="E12" t="n" s="2">
-        <v>0.0145</v>
+        <v>0.0139</v>
       </c>
       <c r="F12" t="n" s="2">
-        <v>0.0162</v>
+        <v>0.01595</v>
       </c>
       <c r="G12" t="n" s="2">
-        <v>0.0170667</v>
+        <v>0.0159</v>
       </c>
     </row>
     <row r="13">
@@ -566,22 +566,22 @@
         <v>10</v>
       </c>
       <c r="B13" t="n" s="2">
-        <v>32.3</v>
+        <v>26.9</v>
       </c>
       <c r="C13" t="n" s="2">
-        <v>17.57</v>
+        <v>16.85</v>
       </c>
       <c r="D13" t="n" s="2">
-        <v>12.198</v>
+        <v>11.912</v>
       </c>
       <c r="E13" t="n" s="2">
-        <v>11.184</v>
+        <v>11.2144</v>
       </c>
       <c r="F13" t="n" s="2">
-        <v>11.2169</v>
+        <v>11.0891</v>
       </c>
       <c r="G13" t="n" s="2">
-        <v>11.171</v>
+        <v>11.1288</v>
       </c>
     </row>
     <row r="14">
@@ -589,22 +589,22 @@
         <v>11</v>
       </c>
       <c r="B14" t="n" s="2">
-        <v>2.6</v>
+        <v>4.9</v>
       </c>
       <c r="C14" t="n" s="2">
-        <v>1.07</v>
+        <v>1.16</v>
       </c>
       <c r="D14" t="n" s="2">
-        <v>0.626</v>
+        <v>0.633</v>
       </c>
       <c r="E14" t="n" s="2">
-        <v>0.5474</v>
+        <v>0.5478</v>
       </c>
       <c r="F14" t="n" s="2">
-        <v>0.5454</v>
+        <v>0.53215</v>
       </c>
       <c r="G14" t="n" s="2">
-        <v>0.540833</v>
+        <v>0.531</v>
       </c>
     </row>
     <row r="15">
@@ -612,22 +612,22 @@
         <v>12</v>
       </c>
       <c r="B15" t="n" s="2">
-        <v>0.3</v>
+        <v>0.7</v>
       </c>
       <c r="C15" t="n" s="2">
-        <v>0.3</v>
+        <v>0.33</v>
       </c>
       <c r="D15" t="n" s="2">
-        <v>0.234</v>
+        <v>0.249</v>
       </c>
       <c r="E15" t="n" s="2">
-        <v>0.1787</v>
+        <v>0.1869</v>
       </c>
       <c r="F15" t="n" s="2">
-        <v>0.16725</v>
+        <v>0.1731</v>
       </c>
       <c r="G15" t="n" s="2">
-        <v>0.1649</v>
+        <v>0.172167</v>
       </c>
     </row>
     <row r="16">
@@ -635,22 +635,22 @@
         <v>13</v>
       </c>
       <c r="B16" t="n" s="2">
-        <v>16.5</v>
+        <v>14.1</v>
       </c>
       <c r="C16" t="n" s="2">
         <v>9.34</v>
       </c>
       <c r="D16" t="n" s="2">
-        <v>6.019</v>
+        <v>6.108</v>
       </c>
       <c r="E16" t="n" s="2">
-        <v>5.459</v>
+        <v>5.6631</v>
       </c>
       <c r="F16" t="n" s="2">
-        <v>5.48955</v>
+        <v>5.5901</v>
       </c>
       <c r="G16" t="n" s="2">
-        <v>5.4785</v>
+        <v>5.61677</v>
       </c>
     </row>
     <row r="17">
@@ -658,22 +658,22 @@
         <v>14</v>
       </c>
       <c r="B17" t="n" s="2">
-        <v>1.0</v>
+        <v>0.8</v>
       </c>
       <c r="C17" t="n" s="2">
-        <v>0.64</v>
+        <v>0.61</v>
       </c>
       <c r="D17" t="n" s="2">
-        <v>0.09</v>
+        <v>0.091</v>
       </c>
       <c r="E17" t="n" s="2">
-        <v>0.0204</v>
+        <v>0.0216</v>
       </c>
       <c r="F17" t="n" s="2">
-        <v>0.01705</v>
+        <v>0.01685</v>
       </c>
       <c r="G17" t="n" s="2">
-        <v>0.0150333</v>
+        <v>0.0153</v>
       </c>
     </row>
   </sheetData>

</xml_diff>